<commit_message>
BalaRaju - Working on PayRoll
</commit_message>
<xml_diff>
--- a/public/Payroll/November-2014-payslips.xlsx
+++ b/public/Payroll/November-2014-payslips.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -75,28 +75,28 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.08988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.88988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.18988764044944"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.989887640449439"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="14.08988764044944"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.78988764044944"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="21.789887640449443"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.589887640449438"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.78988764044944"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="9.68988764044944"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="8.589887640449438"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="12.989887640449439"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="7.489887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -232,17 +232,17 @@
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>Priyanka Muddana</t>
+          <t>fgfg fgfgfg</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>02/06/2014</t>
+          <t>31/12/2014</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>Internship</t>
+          <t>New</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
@@ -256,13 +256,13 @@
         </is>
       </c>
       <c r="H2" s="0" t="n">
-        <v>120000.0</v>
+        <v>12.0</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>10000.0</v>
+        <v>1.0</v>
       </c>
       <c r="J2" s="0" t="n">
-        <v>10345.0</v>
+        <v>0.93</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>30.0</v>
@@ -271,126 +271,40 @@
         <v>30.0</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>4000.0</v>
+        <v>0.4</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>1000.0</v>
+        <v>0.1</v>
       </c>
       <c r="O2" s="0" t="n">
-        <v>4345.0</v>
+        <v>0.43</v>
       </c>
       <c r="P2" s="0" t="n">
-        <v>1000.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q2" s="0" t="n">
-        <v>10345.0</v>
+        <v>0.93</v>
       </c>
       <c r="R2" s="0" t="n">
-        <v>480.0</v>
+        <v>0.05</v>
       </c>
       <c r="S2" s="0" t="n">
-        <v>181.04</v>
+        <v>0.02</v>
       </c>
       <c r="T2" s="0" t="n">
-        <v>150.0</v>
+        <v>0.0</v>
       </c>
       <c r="U2" s="0" t="n">
-        <v>155.0</v>
+        <v>0.0</v>
       </c>
       <c r="V2" s="0" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="W2" s="0" t="n">
-        <v>1066.04</v>
+        <v>0.07</v>
       </c>
       <c r="X2" s="0" t="n">
-        <v>9278.96</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>11-2014</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>Vidya Sagar pogiri</t>
-        </is>
-      </c>
-      <c r="D3" s="0" t="inlineStr">
-        <is>
-          <t>02/06/2014</t>
-        </is>
-      </c>
-      <c r="E3" s="0" t="inlineStr">
-        <is>
-          <t>Regular</t>
-        </is>
-      </c>
-      <c r="F3" s="0" t="inlineStr">
-        <is>
-          <t>Junior Developer</t>
-        </is>
-      </c>
-      <c r="G3" s="0" t="inlineStr">
-        <is>
-          <t>Development</t>
-        </is>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>130000.0</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>10833.333333333334</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>10313.3</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>4333.33</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>1083.33</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <v>4896.67</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q3" s="0" t="n">
-        <v>10313.3</v>
-      </c>
-      <c r="R3" s="0" t="n">
-        <v>520.0</v>
-      </c>
-      <c r="S3" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T3" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U3" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="V3" s="0" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W3" s="0" t="n">
-        <v>520.0</v>
-      </c>
-      <c r="X3" s="0" t="n">
-        <v>9793.33</v>
+        <v>0.86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BalaRaju - Added code
</commit_message>
<xml_diff>
--- a/public/Payroll/November-2014-payslips.xlsx
+++ b/public/Payroll/November-2014-payslips.xlsx
@@ -67,7 +67,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -88,16 +88,17 @@
     <col min="13" max="13" bestFit="true" customWidth="true" width="7.489887640449439"/>
     <col min="14" max="14" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="5.289887640449439"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="5.289887640449439"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="12.989887640449439"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="12.989887640449439"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="7.489887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -178,50 +179,55 @@
       </c>
       <c r="P1" s="0" t="inlineStr">
         <is>
+          <t>fgfg</t>
+        </is>
+      </c>
+      <c r="Q1" s="0" t="inlineStr">
+        <is>
           <t>Spcl Allowance</t>
         </is>
       </c>
-      <c r="Q1" s="0" t="inlineStr">
+      <c r="R1" s="0" t="inlineStr">
         <is>
           <t>Arrears</t>
         </is>
       </c>
-      <c r="R1" s="0" t="inlineStr">
+      <c r="S1" s="0" t="inlineStr">
         <is>
           <t>Gross Pay</t>
         </is>
       </c>
-      <c r="S1" s="0" t="inlineStr">
+      <c r="T1" s="0" t="inlineStr">
         <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="T1" s="0" t="inlineStr">
+      <c r="U1" s="0" t="inlineStr">
         <is>
           <t>ESIC</t>
         </is>
       </c>
-      <c r="U1" s="0" t="inlineStr">
+      <c r="V1" s="0" t="inlineStr">
         <is>
           <t>PT</t>
         </is>
       </c>
-      <c r="V1" s="0" t="inlineStr">
+      <c r="W1" s="0" t="inlineStr">
         <is>
           <t>TDS</t>
         </is>
       </c>
-      <c r="W1" s="0" t="inlineStr">
+      <c r="X1" s="0" t="inlineStr">
         <is>
           <t>Deductible Arrears</t>
         </is>
       </c>
-      <c r="X1" s="0" t="inlineStr">
+      <c r="Y1" s="0" t="inlineStr">
         <is>
           <t>total_deducations</t>
         </is>
       </c>
-      <c r="Y1" s="0" t="inlineStr">
+      <c r="Z1" s="0" t="inlineStr">
         <is>
           <t>NetPay</t>
         </is>
@@ -286,22 +292,22 @@
         <v>0</v>
       </c>
       <c r="P2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="0" t="n">
         <v>0.43</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="R2" s="0" t="n">
         <v>0.0</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="S2" s="0" t="n">
         <v>0.93</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="T2" s="0" t="n">
         <v>0.05</v>
       </c>
-      <c r="T2" s="0" t="n">
+      <c r="U2" s="0" t="n">
         <v>0.02</v>
-      </c>
-      <c r="U2" s="0" t="n">
-        <v>0.0</v>
       </c>
       <c r="V2" s="0" t="n">
         <v>0.0</v>
@@ -310,9 +316,12 @@
         <v>0.0</v>
       </c>
       <c r="X2" s="0" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y2" s="0" t="n">
         <v>0.07</v>
       </c>
-      <c r="Y2" s="0" t="n">
+      <c r="Z2" s="0" t="n">
         <v>0.86</v>
       </c>
     </row>

</xml_diff>